<commit_message>
Correspondence of #12 and, other updates. https://github.com/OpenTouryoProject/OpenTouryoDocuments/issues/12 https://github.com/OpenTouryoProject/OpenTouryoDocuments/issues/19
</commit_message>
<xml_diff>
--- a/documents/document_map.xlsx
+++ b/documents/document_map.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\OTP-OTD\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="408" windowWidth="27792" windowHeight="12276"/>
+    <workbookView xWindow="600" yWindow="405" windowWidth="27795" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
   <si>
     <t>○</t>
     <phoneticPr fontId="1"/>
@@ -249,11 +254,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>御紹介@”棟梁”.pptx
-(Introduction.pptx)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>機能一覧.xls
 (Functional_list.xlsx)</t>
     <phoneticPr fontId="1"/>
@@ -262,8 +262,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -415,7 +415,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -458,19 +458,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" textRotation="180" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -479,6 +482,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -525,7 +536,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,9 +568,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,6 +603,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -766,55 +779,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Y11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="4.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="27.44140625" customWidth="1"/>
-    <col min="2" max="15" width="5.6640625" customWidth="1"/>
-    <col min="16" max="17" width="8.5546875" customWidth="1"/>
-    <col min="18" max="25" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="27.5" customWidth="1"/>
+    <col min="2" max="15" width="5.625" customWidth="1"/>
+    <col min="16" max="16" width="8.5" customWidth="1"/>
+    <col min="17" max="24" width="5.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="42.6" customHeight="1">
+    <row r="1" spans="1:24" ht="42.6" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="19"/>
       <c r="P1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="13" t="s">
+      <c r="Q1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="15"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="18"/>
     </row>
-    <row r="2" spans="1:25" s="1" customFormat="1" ht="362.4" customHeight="1">
+    <row r="2" spans="1:24" s="1" customFormat="1" ht="362.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8" t="s">
         <v>8</v>
       </c>
@@ -857,41 +869,38 @@
       <c r="N2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q2" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>31</v>
       </c>
+      <c r="R2" s="11" t="s">
+        <v>32</v>
+      </c>
       <c r="S2" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="X2" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="21" customHeight="1">
+    <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -908,21 +917,18 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="18"/>
+      <c r="O3" s="15"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="3"/>
+      <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:25" ht="21" customHeight="1">
+    <row r="4" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -939,21 +945,20 @@
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
-      <c r="O4" s="18"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="3"/>
+      <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:25" ht="21" customHeight="1">
+    <row r="5" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -976,19 +981,18 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="18"/>
+      <c r="O5" s="15"/>
       <c r="P5" s="4"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="2"/>
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
       <c r="V5" s="2"/>
       <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="3"/>
+      <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:25" ht="21" customHeight="1">
+    <row r="6" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>11</v>
       </c>
@@ -1031,12 +1035,14 @@
       <c r="N6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O6" s="18" t="s">
+      <c r="O6" s="15" t="s">
         <v>0</v>
       </c>
       <c r="P6" s="4"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="4" t="s">
+      <c r="Q6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="S6" s="2" t="s">
@@ -1054,14 +1060,11 @@
       <c r="W6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="3" t="s">
+      <c r="X6" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="21" customHeight="1">
+    <row r="7" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1100,10 +1103,12 @@
       <c r="N7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O7" s="18"/>
+      <c r="O7" s="15"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="4" t="s">
+      <c r="Q7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="S7" s="2" t="s">
@@ -1121,34 +1126,30 @@
       <c r="W7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="3" t="s">
+      <c r="X7" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="13.5" customHeight="1"/>
-    <row r="9" spans="1:25" ht="21" customHeight="1">
+    <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="21" customHeight="1">
+    <row r="10" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="21" customHeight="1">
+    <row r="11" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="R1:Y1"/>
+  <mergeCells count="2">
+    <mergeCell ref="Q1:X1"/>
     <mergeCell ref="B1:O1"/>
-    <mergeCell ref="P1:Q1"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* Modify the point of pointed out. https://github.com/OpenTouryoProject/OpenTouryoDocuments/pull/20
</commit_message>
<xml_diff>
--- a/documents/document_map.xlsx
+++ b/documents/document_map.xlsx
@@ -261,33 +261,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>△…任意（読むことを推奨するドキュメント） (Any (The document that is recommended to read))</t>
-    <rPh sb="2" eb="4">
-      <t>ニンイ</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="10" eb="12">
-      <t>スイショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>○…必須（読むべきドキュメント） (Required (The document that must be read))</t>
-    <rPh sb="2" eb="4">
-      <t>ヒッス</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>ヨ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>※…特定のアーキテクチャ・機能について書かれているドキュメントは必須（必要に応じて読むべきドキュメント） (Required documents that are written for a specific architecture and function (document should be read if necessary))</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>概要 (Introduction)</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -357,34 +330,6 @@
   </si>
   <si>
     <t>チュートリアル (Tutorial)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2層 C/S C# (2C/S C#)</t>
-    <rPh sb="1" eb="2">
-      <t>ソウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2層 C/S VB (2C/S VB)</t>
-    <rPh sb="1" eb="2">
-      <t>ソウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>3層 C/S C# (3C/S C#)</t>
-    <rPh sb="1" eb="2">
-      <t>ソウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>3層 C/S VB (3C/S VB)</t>
-    <rPh sb="1" eb="2">
-      <t>ソウ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -440,6 +385,61 @@
     <t xml:space="preserve">
 　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　　ロール (Role)
 　　　　ドキュメント (Document)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2層 C/S C# (Two-tier client server application C#)</t>
+    <rPh sb="1" eb="2">
+      <t>ソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2層 C/S VB (Two-tier client server application VB)</t>
+    <rPh sb="1" eb="2">
+      <t>ソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3層 C/S C# (Three-tier client server application C#)</t>
+    <rPh sb="1" eb="2">
+      <t>ソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3層 C/S VB (Three-tier client server application VB)</t>
+    <rPh sb="1" eb="2">
+      <t>ソウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※…特定のアーキテクチャ・機能について書かれているドキュメントは必須（必要に応じて読むべきドキュメント） (It is required to read the documents that describe your architectures or features.)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>△…任意（読むことを推奨するドキュメント） (Not required. (It is recommended to read these documents.))</t>
+    <rPh sb="2" eb="4">
+      <t>ニンイ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>スイショウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>○…必須（読むべきドキュメント） (Required. (It is required to read these documents.))</t>
+    <rPh sb="2" eb="4">
+      <t>ヒッス</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ヨ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -736,6 +736,81 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -764,81 +839,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,10 +1147,10 @@
   <dimension ref="A1:L98"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="B79" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1167,7 +1167,7 @@
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="6"/>
       <c r="B1" s="7" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1182,7 +1182,7 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -1197,7 +1197,7 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="6"/>
       <c r="B3" s="7" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
@@ -1210,172 +1210,172 @@
       <c r="K3" s="10"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A4" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="38" t="s">
+      <c r="A4" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="39"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A5" s="11"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="39" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="27"/>
+      <c r="H5" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A6" s="11"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="38" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A7" s="11"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="38" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="25"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A8" s="11"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25" t="s">
         <v>62</v>
       </c>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A9" s="21">
+      <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="26"/>
+      <c r="B9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A10" s="21">
+      <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="26"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A11" s="21">
+      <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="32" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
+      <c r="K11" s="33"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A12" s="21">
+      <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="31" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="34"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A13" s="21">
+      <c r="A13" s="11">
         <v>5</v>
       </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="31" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="21" t="s">
         <v>9</v>
       </c>
       <c r="G13" s="35"/>
@@ -1385,54 +1385,54 @@
       <c r="K13" s="35"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A14" s="21">
+      <c r="A14" s="11">
         <v>6</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A15" s="21">
+      <c r="A15" s="11">
         <v>7</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="E15" s="31" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="34"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A16" s="21">
+      <c r="A16" s="11">
         <v>8</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="31" t="s">
+      <c r="B16" s="23"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="21" t="s">
         <v>4</v>
       </c>
       <c r="G16" s="35"/>
@@ -1442,92 +1442,92 @@
       <c r="K16" s="35"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A17" s="21">
+      <c r="A17" s="11">
         <v>9</v>
       </c>
-      <c r="B17" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="26"/>
+      <c r="B17" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="16"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A18" s="21">
+      <c r="A18" s="11">
         <v>10</v>
       </c>
-      <c r="B18" s="27"/>
-      <c r="C18" s="28" t="s">
+      <c r="B18" s="17"/>
+      <c r="C18" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="26"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="16"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A19" s="21">
+      <c r="A19" s="11">
         <v>11</v>
       </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32" t="s">
+      <c r="B19" s="17"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="32" t="s">
+      <c r="I19" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J19" s="32" t="s">
+      <c r="J19" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K19" s="32"/>
+      <c r="K19" s="33"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A20" s="21">
+      <c r="A20" s="11">
         <v>12</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="31" t="s">
+      <c r="B20" s="17"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G20" s="33"/>
-      <c r="H20" s="33"/>
-      <c r="I20" s="33"/>
-      <c r="J20" s="33"/>
-      <c r="K20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A21" s="21">
+      <c r="A21" s="11">
         <v>13</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="31" t="s">
+      <c r="B21" s="17"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="21" t="s">
         <v>12</v>
       </c>
       <c r="G21" s="35"/>
@@ -1537,58 +1537,58 @@
       <c r="K21" s="35"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A22" s="21">
+      <c r="A22" s="11">
         <v>14</v>
       </c>
-      <c r="B22" s="27"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J22" s="32" t="s">
+      <c r="J22" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="K22" s="33" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A23" s="21">
+      <c r="A23" s="11">
         <v>15</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="31" t="s">
+      <c r="B23" s="17"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A24" s="21">
+      <c r="A24" s="11">
         <v>16</v>
       </c>
-      <c r="B24" s="27"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="31" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="21" t="s">
         <v>13</v>
       </c>
       <c r="G24" s="35"/>
@@ -1598,58 +1598,58 @@
       <c r="K24" s="35"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A25" s="21">
+      <c r="A25" s="11">
         <v>17</v>
       </c>
-      <c r="B25" s="27"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32" t="s">
+      <c r="B25" s="17"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J25" s="32" t="s">
+      <c r="J25" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K25" s="32" t="s">
+      <c r="K25" s="33" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A26" s="21">
+      <c r="A26" s="11">
         <v>18</v>
       </c>
-      <c r="B26" s="27"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="31" t="s">
+      <c r="B26" s="17"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
-      <c r="J26" s="33"/>
-      <c r="K26" s="33"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A27" s="21">
+      <c r="A27" s="11">
         <v>19</v>
       </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="31" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="31" t="s">
+      <c r="F27" s="21" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="35"/>
@@ -1659,56 +1659,56 @@
       <c r="K27" s="35"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A28" s="21">
+      <c r="A28" s="11">
         <v>20</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="K28" s="32" t="s">
+      <c r="K28" s="33" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A29" s="21">
+      <c r="A29" s="11">
         <v>21</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="31" t="s">
+      <c r="B29" s="17"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="31" t="s">
+      <c r="F29" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G29" s="33"/>
-      <c r="H29" s="33"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="33"/>
-      <c r="K29" s="33"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A30" s="21">
+      <c r="A30" s="11">
         <v>22</v>
       </c>
-      <c r="B30" s="27"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="31" t="s">
+      <c r="B30" s="17"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="21" t="s">
         <v>17</v>
       </c>
       <c r="G30" s="35"/>
@@ -1718,56 +1718,56 @@
       <c r="K30" s="35"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A31" s="21">
+      <c r="A31" s="11">
         <v>23</v>
       </c>
-      <c r="B31" s="27"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
-      <c r="I31" s="32" t="s">
+      <c r="B31" s="17"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J31" s="32" t="s">
+      <c r="J31" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K31" s="32"/>
+      <c r="K31" s="33"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A32" s="21">
+      <c r="A32" s="11">
         <v>24</v>
       </c>
-      <c r="B32" s="27"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="31" t="s">
+      <c r="B32" s="17"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
-      <c r="J32" s="33"/>
-      <c r="K32" s="33"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A33" s="21">
+      <c r="A33" s="11">
         <v>25</v>
       </c>
-      <c r="B33" s="27"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="31" t="s">
+      <c r="B33" s="17"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="21" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="35"/>
@@ -1777,56 +1777,56 @@
       <c r="K33" s="35"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A34" s="21">
+      <c r="A34" s="11">
         <v>26</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="32" t="s">
+      <c r="B34" s="17"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="33"/>
+      <c r="H34" s="33"/>
+      <c r="I34" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J34" s="32" t="s">
+      <c r="J34" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K34" s="32"/>
+      <c r="K34" s="33"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A35" s="21">
+      <c r="A35" s="11">
         <v>27</v>
       </c>
-      <c r="B35" s="27"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="31" t="s">
+      <c r="B35" s="17"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="33"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="34"/>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="34"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A36" s="21">
+      <c r="A36" s="11">
         <v>28</v>
       </c>
-      <c r="B36" s="27"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="31" t="s">
+      <c r="B36" s="17"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="21" t="s">
         <v>19</v>
       </c>
       <c r="G36" s="35"/>
@@ -1836,52 +1836,52 @@
       <c r="K36" s="35"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A37" s="21">
+      <c r="A37" s="11">
         <v>29</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32" t="s">
+      <c r="B37" s="17"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K37" s="32" t="s">
+      <c r="K37" s="33" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A38" s="21">
+      <c r="A38" s="11">
         <v>30</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="31" t="s">
+      <c r="B38" s="17"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G38" s="33"/>
-      <c r="H38" s="33"/>
-      <c r="I38" s="33"/>
-      <c r="J38" s="33"/>
-      <c r="K38" s="33"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="34"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="34"/>
+      <c r="K38" s="34"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A39" s="21">
+      <c r="A39" s="11">
         <v>31</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="31" t="s">
+      <c r="B39" s="17"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21" t="s">
         <v>21</v>
       </c>
       <c r="G39" s="35"/>
@@ -1891,56 +1891,56 @@
       <c r="K39" s="35"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A40" s="21">
+      <c r="A40" s="11">
         <v>32</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="29"/>
-      <c r="D40" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="32" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K40" s="32" t="s">
+      <c r="K40" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A41" s="21">
+      <c r="A41" s="11">
         <v>33</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="29"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="31" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="33"/>
-      <c r="H41" s="33"/>
-      <c r="I41" s="33"/>
-      <c r="J41" s="33"/>
-      <c r="K41" s="33"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A42" s="21">
+      <c r="A42" s="11">
         <v>34</v>
       </c>
-      <c r="B42" s="27"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="31" t="s">
+      <c r="B42" s="17"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="21" t="s">
         <v>23</v>
       </c>
       <c r="G42" s="35"/>
@@ -1950,56 +1950,56 @@
       <c r="K42" s="35"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A43" s="21">
+      <c r="A43" s="11">
         <v>35</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="29"/>
-      <c r="D43" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="E43" s="31"/>
-      <c r="F43" s="31"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
-      <c r="I43" s="32"/>
-      <c r="J43" s="32" t="s">
+      <c r="B43" s="17"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="33"/>
+      <c r="J43" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K43" s="32" t="s">
+      <c r="K43" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A44" s="21">
+      <c r="A44" s="11">
         <v>36</v>
       </c>
-      <c r="B44" s="27"/>
-      <c r="C44" s="29"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="31" t="s">
+      <c r="B44" s="17"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A45" s="21">
+      <c r="A45" s="11">
         <v>37</v>
       </c>
-      <c r="B45" s="27"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="31" t="s">
+      <c r="B45" s="17"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="22"/>
+      <c r="E45" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="21" t="s">
         <v>25</v>
       </c>
       <c r="G45" s="35"/>
@@ -2009,56 +2009,56 @@
       <c r="K45" s="35"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A46" s="21">
+      <c r="A46" s="11">
         <v>38</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="29"/>
-      <c r="D46" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
-      <c r="I46" s="32"/>
-      <c r="J46" s="32" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="33"/>
+      <c r="H46" s="33"/>
+      <c r="I46" s="33"/>
+      <c r="J46" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K46" s="32" t="s">
+      <c r="K46" s="33" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A47" s="21">
+      <c r="A47" s="11">
         <v>39</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="29"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="31" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G47" s="33"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="33"/>
-      <c r="J47" s="33"/>
-      <c r="K47" s="33"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="34"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A48" s="21">
+      <c r="A48" s="11">
         <v>40</v>
       </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="29"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="31" t="s">
+      <c r="B48" s="17"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F48" s="21" t="s">
         <v>27</v>
       </c>
       <c r="G48" s="35"/>
@@ -2068,56 +2068,56 @@
       <c r="K48" s="35"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A49" s="21">
+      <c r="A49" s="11">
         <v>41</v>
       </c>
-      <c r="B49" s="27"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
-      <c r="I49" s="32"/>
-      <c r="J49" s="32" t="s">
+      <c r="B49" s="17"/>
+      <c r="C49" s="19"/>
+      <c r="D49" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="33"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K49" s="32" t="s">
+      <c r="K49" s="33" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A50" s="21">
+      <c r="A50" s="11">
         <v>42</v>
       </c>
-      <c r="B50" s="27"/>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="31" t="s">
+      <c r="B50" s="17"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F50" s="31" t="s">
+      <c r="F50" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G50" s="33"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="33"/>
-      <c r="J50" s="33"/>
-      <c r="K50" s="33"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A51" s="21">
+      <c r="A51" s="11">
         <v>43</v>
       </c>
-      <c r="B51" s="27"/>
-      <c r="C51" s="29"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="31" t="s">
+      <c r="B51" s="17"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F51" s="31" t="s">
+      <c r="F51" s="21" t="s">
         <v>29</v>
       </c>
       <c r="G51" s="35"/>
@@ -2127,56 +2127,56 @@
       <c r="K51" s="35"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A52" s="21">
+      <c r="A52" s="11">
         <v>44</v>
       </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="E52" s="31"/>
-      <c r="F52" s="31"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32" t="s">
+      <c r="B52" s="17"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K52" s="32" t="s">
+      <c r="K52" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A53" s="21">
+      <c r="A53" s="11">
         <v>45</v>
       </c>
-      <c r="B53" s="27"/>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="31" t="s">
+      <c r="B53" s="17"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F53" s="31" t="s">
+      <c r="F53" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G53" s="33"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="33"/>
-      <c r="J53" s="33"/>
-      <c r="K53" s="33"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A54" s="21">
+      <c r="A54" s="11">
         <v>46</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="29"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="31" t="s">
+      <c r="B54" s="17"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F54" s="21" t="s">
         <v>31</v>
       </c>
       <c r="G54" s="35"/>
@@ -2186,56 +2186,56 @@
       <c r="K54" s="35"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A55" s="21">
+      <c r="A55" s="11">
         <v>47</v>
       </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="29"/>
-      <c r="D55" s="30" t="s">
-        <v>80</v>
-      </c>
-      <c r="E55" s="31"/>
-      <c r="F55" s="31"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
-      <c r="I55" s="32"/>
-      <c r="J55" s="32" t="s">
+      <c r="B55" s="17"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E55" s="21"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="33"/>
+      <c r="J55" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K55" s="32" t="s">
+      <c r="K55" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A56" s="21">
+      <c r="A56" s="11">
         <v>48</v>
       </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="29"/>
-      <c r="E56" s="31" t="s">
+      <c r="B56" s="17"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="33"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="34"/>
+      <c r="I56" s="34"/>
+      <c r="J56" s="34"/>
+      <c r="K56" s="34"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A57" s="21">
+      <c r="A57" s="11">
         <v>49</v>
       </c>
-      <c r="B57" s="36"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="31" t="s">
+      <c r="B57" s="23"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F57" s="21" t="s">
         <v>32</v>
       </c>
       <c r="G57" s="35"/>
@@ -2245,90 +2245,90 @@
       <c r="K57" s="35"/>
     </row>
     <row r="58" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="21">
+      <c r="A58" s="11">
         <v>50</v>
       </c>
-      <c r="B58" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C58" s="23"/>
-      <c r="D58" s="23"/>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="25"/>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="26"/>
+      <c r="B58" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="15"/>
+      <c r="H58" s="15"/>
+      <c r="I58" s="15"/>
+      <c r="J58" s="15"/>
+      <c r="K58" s="16"/>
     </row>
     <row r="59" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="21">
+      <c r="A59" s="11">
         <v>51</v>
       </c>
-      <c r="B59" s="27"/>
-      <c r="C59" s="28" t="s">
+      <c r="B59" s="17"/>
+      <c r="C59" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D59" s="23"/>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="25"/>
-      <c r="H59" s="25"/>
-      <c r="I59" s="25"/>
-      <c r="J59" s="25"/>
-      <c r="K59" s="26"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="16"/>
     </row>
     <row r="60" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="21">
+      <c r="A60" s="11">
         <v>52</v>
       </c>
-      <c r="B60" s="27"/>
-      <c r="C60" s="29"/>
-      <c r="D60" s="30" t="s">
+      <c r="B60" s="17"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
-      <c r="I60" s="32"/>
-      <c r="J60" s="32" t="s">
+      <c r="E60" s="21"/>
+      <c r="F60" s="21"/>
+      <c r="G60" s="33"/>
+      <c r="H60" s="33"/>
+      <c r="I60" s="33"/>
+      <c r="J60" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K60" s="32" t="s">
+      <c r="K60" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="21">
+      <c r="A61" s="11">
         <v>53</v>
       </c>
-      <c r="B61" s="27"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="29"/>
-      <c r="E61" s="31" t="s">
+      <c r="B61" s="17"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F61" s="31" t="s">
+      <c r="F61" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="33"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="34"/>
+      <c r="I61" s="34"/>
+      <c r="J61" s="34"/>
+      <c r="K61" s="34"/>
     </row>
     <row r="62" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="21">
+      <c r="A62" s="11">
         <v>54</v>
       </c>
-      <c r="B62" s="27"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="31" t="s">
+      <c r="B62" s="17"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F62" s="31" t="s">
+      <c r="F62" s="21" t="s">
         <v>33</v>
       </c>
       <c r="G62" s="35"/>
@@ -2338,56 +2338,56 @@
       <c r="K62" s="35"/>
     </row>
     <row r="63" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="21">
+      <c r="A63" s="11">
         <v>55</v>
       </c>
-      <c r="B63" s="27"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="30" t="s">
+      <c r="B63" s="17"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="E63" s="31"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="32"/>
-      <c r="I63" s="32"/>
-      <c r="J63" s="32" t="s">
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="33"/>
+      <c r="H63" s="33"/>
+      <c r="I63" s="33"/>
+      <c r="J63" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K63" s="32" t="s">
+      <c r="K63" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="21">
+      <c r="A64" s="11">
         <v>56</v>
       </c>
-      <c r="B64" s="27"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="29"/>
-      <c r="E64" s="31" t="s">
+      <c r="B64" s="17"/>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F64" s="31" t="s">
+      <c r="F64" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="33"/>
-      <c r="H64" s="33"/>
-      <c r="I64" s="33"/>
-      <c r="J64" s="33"/>
-      <c r="K64" s="33"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="34"/>
+      <c r="J64" s="34"/>
+      <c r="K64" s="34"/>
     </row>
     <row r="65" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="21">
+      <c r="A65" s="11">
         <v>57</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="29"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="31" t="s">
+      <c r="B65" s="17"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F65" s="31" t="s">
+      <c r="F65" s="21" t="s">
         <v>37</v>
       </c>
       <c r="G65" s="35"/>
@@ -2397,56 +2397,56 @@
       <c r="K65" s="35"/>
     </row>
     <row r="66" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="21">
+      <c r="A66" s="11">
         <v>58</v>
       </c>
-      <c r="B66" s="27"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="30" t="s">
+      <c r="B66" s="17"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="31"/>
-      <c r="F66" s="31"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="32" t="s">
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K66" s="32" t="s">
+      <c r="K66" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="21">
+      <c r="A67" s="11">
         <v>59</v>
       </c>
-      <c r="B67" s="27"/>
-      <c r="C67" s="29"/>
-      <c r="D67" s="29"/>
-      <c r="E67" s="31" t="s">
+      <c r="B67" s="17"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F67" s="31" t="s">
+      <c r="F67" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G67" s="33"/>
-      <c r="H67" s="33"/>
-      <c r="I67" s="33"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="33"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="34"/>
+      <c r="I67" s="34"/>
+      <c r="J67" s="34"/>
+      <c r="K67" s="34"/>
     </row>
     <row r="68" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="21">
+      <c r="A68" s="11">
         <v>60</v>
       </c>
-      <c r="B68" s="27"/>
-      <c r="C68" s="29"/>
-      <c r="D68" s="34"/>
-      <c r="E68" s="31" t="s">
+      <c r="B68" s="17"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F68" s="31" t="s">
+      <c r="F68" s="21" t="s">
         <v>48</v>
       </c>
       <c r="G68" s="35"/>
@@ -2456,56 +2456,56 @@
       <c r="K68" s="35"/>
     </row>
     <row r="69" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="21">
+      <c r="A69" s="11">
         <v>61</v>
       </c>
-      <c r="B69" s="27"/>
-      <c r="C69" s="29"/>
-      <c r="D69" s="30" t="s">
+      <c r="B69" s="17"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="32"/>
-      <c r="I69" s="32"/>
-      <c r="J69" s="32" t="s">
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="33"/>
+      <c r="I69" s="33"/>
+      <c r="J69" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K69" s="32" t="s">
+      <c r="K69" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="21">
+      <c r="A70" s="11">
         <v>62</v>
       </c>
-      <c r="B70" s="27"/>
-      <c r="C70" s="29"/>
-      <c r="D70" s="29"/>
-      <c r="E70" s="31" t="s">
+      <c r="B70" s="17"/>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="F70" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="G70" s="33"/>
-      <c r="H70" s="33"/>
-      <c r="I70" s="33"/>
-      <c r="J70" s="33"/>
-      <c r="K70" s="33"/>
+      <c r="G70" s="34"/>
+      <c r="H70" s="34"/>
+      <c r="I70" s="34"/>
+      <c r="J70" s="34"/>
+      <c r="K70" s="34"/>
     </row>
     <row r="71" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="21">
+      <c r="A71" s="11">
         <v>63</v>
       </c>
-      <c r="B71" s="27"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="34"/>
-      <c r="E71" s="31" t="s">
+      <c r="B71" s="17"/>
+      <c r="C71" s="19"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F71" s="31" t="s">
+      <c r="F71" s="21" t="s">
         <v>6</v>
       </c>
       <c r="G71" s="35"/>
@@ -2515,56 +2515,56 @@
       <c r="K71" s="35"/>
     </row>
     <row r="72" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="21">
+      <c r="A72" s="11">
         <v>64</v>
       </c>
-      <c r="B72" s="27"/>
-      <c r="C72" s="29"/>
-      <c r="D72" s="30" t="s">
-        <v>84</v>
-      </c>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="32"/>
-      <c r="I72" s="32"/>
-      <c r="J72" s="32" t="s">
+      <c r="B72" s="17"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E72" s="21"/>
+      <c r="F72" s="21"/>
+      <c r="G72" s="33"/>
+      <c r="H72" s="33"/>
+      <c r="I72" s="33"/>
+      <c r="J72" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K72" s="32" t="s">
+      <c r="K72" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="21">
+      <c r="A73" s="11">
         <v>65</v>
       </c>
-      <c r="B73" s="27"/>
-      <c r="C73" s="29"/>
-      <c r="D73" s="29"/>
-      <c r="E73" s="31" t="s">
+      <c r="B73" s="17"/>
+      <c r="C73" s="19"/>
+      <c r="D73" s="19"/>
+      <c r="E73" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F73" s="31" t="s">
+      <c r="F73" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G73" s="33"/>
-      <c r="H73" s="33"/>
-      <c r="I73" s="33"/>
-      <c r="J73" s="33"/>
-      <c r="K73" s="33"/>
+      <c r="G73" s="34"/>
+      <c r="H73" s="34"/>
+      <c r="I73" s="34"/>
+      <c r="J73" s="34"/>
+      <c r="K73" s="34"/>
     </row>
     <row r="74" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="21">
+      <c r="A74" s="11">
         <v>66</v>
       </c>
-      <c r="B74" s="27"/>
-      <c r="C74" s="29"/>
-      <c r="D74" s="34"/>
-      <c r="E74" s="31" t="s">
+      <c r="B74" s="17"/>
+      <c r="C74" s="19"/>
+      <c r="D74" s="22"/>
+      <c r="E74" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F74" s="31" t="s">
+      <c r="F74" s="21" t="s">
         <v>40</v>
       </c>
       <c r="G74" s="35"/>
@@ -2574,56 +2574,56 @@
       <c r="K74" s="35"/>
     </row>
     <row r="75" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="21">
+      <c r="A75" s="11">
         <v>67</v>
       </c>
-      <c r="B75" s="27"/>
-      <c r="C75" s="29"/>
-      <c r="D75" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-      <c r="G75" s="32"/>
-      <c r="H75" s="32"/>
-      <c r="I75" s="32"/>
-      <c r="J75" s="32" t="s">
+      <c r="B75" s="17"/>
+      <c r="C75" s="19"/>
+      <c r="D75" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="33"/>
+      <c r="I75" s="33"/>
+      <c r="J75" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K75" s="32" t="s">
+      <c r="K75" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="21">
+      <c r="A76" s="11">
         <v>68</v>
       </c>
-      <c r="B76" s="27"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="29"/>
-      <c r="E76" s="31" t="s">
+      <c r="B76" s="17"/>
+      <c r="C76" s="19"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="31" t="s">
+      <c r="F76" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G76" s="33"/>
-      <c r="H76" s="33"/>
-      <c r="I76" s="33"/>
-      <c r="J76" s="33"/>
-      <c r="K76" s="33"/>
+      <c r="G76" s="34"/>
+      <c r="H76" s="34"/>
+      <c r="I76" s="34"/>
+      <c r="J76" s="34"/>
+      <c r="K76" s="34"/>
     </row>
     <row r="77" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="21">
+      <c r="A77" s="11">
         <v>69</v>
       </c>
-      <c r="B77" s="27"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="31" t="s">
+      <c r="B77" s="17"/>
+      <c r="C77" s="19"/>
+      <c r="D77" s="22"/>
+      <c r="E77" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F77" s="31" t="s">
+      <c r="F77" s="21" t="s">
         <v>39</v>
       </c>
       <c r="G77" s="35"/>
@@ -2633,56 +2633,56 @@
       <c r="K77" s="35"/>
     </row>
     <row r="78" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="21">
+      <c r="A78" s="11">
         <v>70</v>
       </c>
-      <c r="B78" s="27"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="30" t="s">
-        <v>86</v>
-      </c>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
-      <c r="G78" s="32"/>
-      <c r="H78" s="32"/>
-      <c r="I78" s="32"/>
-      <c r="J78" s="32" t="s">
+      <c r="B78" s="17"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="33"/>
+      <c r="I78" s="33"/>
+      <c r="J78" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K78" s="32" t="s">
+      <c r="K78" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="21">
+      <c r="A79" s="11">
         <v>71</v>
       </c>
-      <c r="B79" s="27"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="31" t="s">
+      <c r="B79" s="17"/>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F79" s="31" t="s">
+      <c r="F79" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="G79" s="33"/>
-      <c r="H79" s="33"/>
-      <c r="I79" s="33"/>
-      <c r="J79" s="33"/>
-      <c r="K79" s="33"/>
+      <c r="G79" s="34"/>
+      <c r="H79" s="34"/>
+      <c r="I79" s="34"/>
+      <c r="J79" s="34"/>
+      <c r="K79" s="34"/>
     </row>
     <row r="80" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="21">
+      <c r="A80" s="11">
         <v>72</v>
       </c>
-      <c r="B80" s="27"/>
-      <c r="C80" s="29"/>
-      <c r="D80" s="34"/>
-      <c r="E80" s="31" t="s">
+      <c r="B80" s="17"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F80" s="31" t="s">
+      <c r="F80" s="21" t="s">
         <v>43</v>
       </c>
       <c r="G80" s="35"/>
@@ -2692,56 +2692,56 @@
       <c r="K80" s="35"/>
     </row>
     <row r="81" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="21">
+      <c r="A81" s="11">
         <v>73</v>
       </c>
-      <c r="B81" s="27"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E81" s="31"/>
-      <c r="F81" s="31"/>
-      <c r="G81" s="32"/>
-      <c r="H81" s="32"/>
-      <c r="I81" s="32"/>
-      <c r="J81" s="32" t="s">
+      <c r="B81" s="17"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="33"/>
+      <c r="H81" s="33"/>
+      <c r="I81" s="33"/>
+      <c r="J81" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K81" s="32" t="s">
+      <c r="K81" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="21">
+      <c r="A82" s="11">
         <v>74</v>
       </c>
-      <c r="B82" s="27"/>
-      <c r="C82" s="29"/>
-      <c r="D82" s="29"/>
-      <c r="E82" s="31" t="s">
+      <c r="B82" s="17"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F82" s="31" t="s">
+      <c r="F82" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G82" s="33"/>
-      <c r="H82" s="33"/>
-      <c r="I82" s="33"/>
-      <c r="J82" s="33"/>
-      <c r="K82" s="33"/>
+      <c r="G82" s="34"/>
+      <c r="H82" s="34"/>
+      <c r="I82" s="34"/>
+      <c r="J82" s="34"/>
+      <c r="K82" s="34"/>
     </row>
     <row r="83" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="21">
+      <c r="A83" s="11">
         <v>75</v>
       </c>
-      <c r="B83" s="27"/>
-      <c r="C83" s="29"/>
-      <c r="D83" s="34"/>
-      <c r="E83" s="31" t="s">
+      <c r="B83" s="17"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="22"/>
+      <c r="E83" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F83" s="31" t="s">
+      <c r="F83" s="21" t="s">
         <v>44</v>
       </c>
       <c r="G83" s="35"/>
@@ -2751,56 +2751,56 @@
       <c r="K83" s="35"/>
     </row>
     <row r="84" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="21">
+      <c r="A84" s="11">
         <v>76</v>
       </c>
-      <c r="B84" s="27"/>
-      <c r="C84" s="29"/>
-      <c r="D84" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="E84" s="31"/>
-      <c r="F84" s="31"/>
-      <c r="G84" s="32"/>
-      <c r="H84" s="32"/>
-      <c r="I84" s="32"/>
-      <c r="J84" s="32" t="s">
+      <c r="B84" s="17"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E84" s="21"/>
+      <c r="F84" s="21"/>
+      <c r="G84" s="33"/>
+      <c r="H84" s="33"/>
+      <c r="I84" s="33"/>
+      <c r="J84" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K84" s="32" t="s">
+      <c r="K84" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="21">
+      <c r="A85" s="11">
         <v>77</v>
       </c>
-      <c r="B85" s="27"/>
-      <c r="C85" s="29"/>
-      <c r="D85" s="29"/>
-      <c r="E85" s="31" t="s">
+      <c r="B85" s="17"/>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F85" s="30" t="s">
+      <c r="F85" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G85" s="33"/>
-      <c r="H85" s="33"/>
-      <c r="I85" s="33"/>
-      <c r="J85" s="33"/>
-      <c r="K85" s="33"/>
+      <c r="G85" s="34"/>
+      <c r="H85" s="34"/>
+      <c r="I85" s="34"/>
+      <c r="J85" s="34"/>
+      <c r="K85" s="34"/>
     </row>
     <row r="86" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="21">
+      <c r="A86" s="11">
         <v>78</v>
       </c>
-      <c r="B86" s="27"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="34"/>
-      <c r="E86" s="31" t="s">
+      <c r="B86" s="17"/>
+      <c r="C86" s="19"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F86" s="30" t="s">
+      <c r="F86" s="20" t="s">
         <v>51</v>
       </c>
       <c r="G86" s="35"/>
@@ -2810,56 +2810,56 @@
       <c r="K86" s="35"/>
     </row>
     <row r="87" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="21">
+      <c r="A87" s="11">
         <v>79</v>
       </c>
-      <c r="B87" s="27"/>
-      <c r="C87" s="29"/>
-      <c r="D87" s="30" t="s">
-        <v>89</v>
-      </c>
-      <c r="E87" s="31"/>
-      <c r="F87" s="31"/>
-      <c r="G87" s="32"/>
-      <c r="H87" s="32"/>
-      <c r="I87" s="32"/>
-      <c r="J87" s="32" t="s">
+      <c r="B87" s="17"/>
+      <c r="C87" s="19"/>
+      <c r="D87" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E87" s="21"/>
+      <c r="F87" s="21"/>
+      <c r="G87" s="33"/>
+      <c r="H87" s="33"/>
+      <c r="I87" s="33"/>
+      <c r="J87" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K87" s="32" t="s">
+      <c r="K87" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="21">
+      <c r="A88" s="11">
         <v>80</v>
       </c>
-      <c r="B88" s="27"/>
-      <c r="C88" s="29"/>
-      <c r="D88" s="29"/>
-      <c r="E88" s="31" t="s">
+      <c r="B88" s="17"/>
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F88" s="31" t="s">
+      <c r="F88" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="G88" s="33"/>
-      <c r="H88" s="33"/>
-      <c r="I88" s="33"/>
-      <c r="J88" s="33"/>
-      <c r="K88" s="33"/>
+      <c r="G88" s="34"/>
+      <c r="H88" s="34"/>
+      <c r="I88" s="34"/>
+      <c r="J88" s="34"/>
+      <c r="K88" s="34"/>
     </row>
     <row r="89" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="21">
+      <c r="A89" s="11">
         <v>81</v>
       </c>
-      <c r="B89" s="27"/>
-      <c r="C89" s="29"/>
-      <c r="D89" s="34"/>
-      <c r="E89" s="31" t="s">
+      <c r="B89" s="17"/>
+      <c r="C89" s="19"/>
+      <c r="D89" s="22"/>
+      <c r="E89" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F89" s="31" t="s">
+      <c r="F89" s="21" t="s">
         <v>56</v>
       </c>
       <c r="G89" s="35"/>
@@ -2869,56 +2869,56 @@
       <c r="K89" s="35"/>
     </row>
     <row r="90" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="21">
+      <c r="A90" s="11">
         <v>82</v>
       </c>
-      <c r="B90" s="27"/>
-      <c r="C90" s="29"/>
-      <c r="D90" s="30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E90" s="31"/>
-      <c r="F90" s="31"/>
-      <c r="G90" s="32"/>
-      <c r="H90" s="32"/>
-      <c r="I90" s="32"/>
-      <c r="J90" s="32" t="s">
+      <c r="B90" s="17"/>
+      <c r="C90" s="19"/>
+      <c r="D90" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="33"/>
+      <c r="H90" s="33"/>
+      <c r="I90" s="33"/>
+      <c r="J90" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="K90" s="32" t="s">
+      <c r="K90" s="33" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="21">
+      <c r="A91" s="11">
         <v>83</v>
       </c>
-      <c r="B91" s="27"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="29"/>
-      <c r="E91" s="31" t="s">
+      <c r="B91" s="17"/>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F91" s="31" t="s">
+      <c r="F91" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="G91" s="33"/>
-      <c r="H91" s="33"/>
-      <c r="I91" s="33"/>
-      <c r="J91" s="33"/>
-      <c r="K91" s="33"/>
+      <c r="G91" s="34"/>
+      <c r="H91" s="34"/>
+      <c r="I91" s="34"/>
+      <c r="J91" s="34"/>
+      <c r="K91" s="34"/>
     </row>
     <row r="92" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="21">
+      <c r="A92" s="11">
         <v>84</v>
       </c>
-      <c r="B92" s="27"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="34"/>
-      <c r="E92" s="31" t="s">
+      <c r="B92" s="17"/>
+      <c r="C92" s="19"/>
+      <c r="D92" s="22"/>
+      <c r="E92" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F92" s="31" t="s">
+      <c r="F92" s="21" t="s">
         <v>6</v>
       </c>
       <c r="G92" s="35"/>
@@ -2928,56 +2928,56 @@
       <c r="K92" s="35"/>
     </row>
     <row r="93" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="21">
+      <c r="A93" s="11">
         <v>85</v>
       </c>
-      <c r="B93" s="27"/>
-      <c r="C93" s="29"/>
-      <c r="D93" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="E93" s="31"/>
-      <c r="F93" s="31"/>
-      <c r="G93" s="32"/>
-      <c r="H93" s="32"/>
-      <c r="I93" s="32" t="s">
+      <c r="B93" s="17"/>
+      <c r="C93" s="19"/>
+      <c r="D93" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="33"/>
+      <c r="H93" s="33"/>
+      <c r="I93" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J93" s="32" t="s">
+      <c r="J93" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K93" s="32"/>
+      <c r="K93" s="33"/>
     </row>
     <row r="94" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="21">
+      <c r="A94" s="11">
         <v>86</v>
       </c>
-      <c r="B94" s="27"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="31" t="s">
+      <c r="B94" s="17"/>
+      <c r="C94" s="19"/>
+      <c r="D94" s="19"/>
+      <c r="E94" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F94" s="31" t="s">
+      <c r="F94" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="G94" s="33"/>
-      <c r="H94" s="33"/>
-      <c r="I94" s="33"/>
-      <c r="J94" s="33"/>
-      <c r="K94" s="33"/>
+      <c r="G94" s="34"/>
+      <c r="H94" s="34"/>
+      <c r="I94" s="34"/>
+      <c r="J94" s="34"/>
+      <c r="K94" s="34"/>
     </row>
     <row r="95" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="21">
+      <c r="A95" s="11">
         <v>87</v>
       </c>
-      <c r="B95" s="27"/>
-      <c r="C95" s="29"/>
-      <c r="D95" s="34"/>
-      <c r="E95" s="31" t="s">
+      <c r="B95" s="17"/>
+      <c r="C95" s="19"/>
+      <c r="D95" s="22"/>
+      <c r="E95" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F95" s="31" t="s">
+      <c r="F95" s="21" t="s">
         <v>52</v>
       </c>
       <c r="G95" s="35"/>
@@ -2987,56 +2987,56 @@
       <c r="K95" s="35"/>
     </row>
     <row r="96" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="21">
+      <c r="A96" s="11">
         <v>88</v>
       </c>
-      <c r="B96" s="27"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96" s="31"/>
-      <c r="F96" s="31"/>
-      <c r="G96" s="32"/>
-      <c r="H96" s="32"/>
-      <c r="I96" s="32" t="s">
+      <c r="B96" s="17"/>
+      <c r="C96" s="19"/>
+      <c r="D96" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="E96" s="21"/>
+      <c r="F96" s="21"/>
+      <c r="G96" s="33"/>
+      <c r="H96" s="33"/>
+      <c r="I96" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="J96" s="32" t="s">
+      <c r="J96" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="K96" s="32"/>
+      <c r="K96" s="33"/>
     </row>
     <row r="97" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="21">
+      <c r="A97" s="11">
         <v>89</v>
       </c>
-      <c r="B97" s="27"/>
-      <c r="C97" s="29"/>
-      <c r="D97" s="29"/>
-      <c r="E97" s="31" t="s">
+      <c r="B97" s="17"/>
+      <c r="C97" s="19"/>
+      <c r="D97" s="19"/>
+      <c r="E97" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="F97" s="31" t="s">
+      <c r="F97" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="G97" s="33"/>
-      <c r="H97" s="33"/>
-      <c r="I97" s="33"/>
-      <c r="J97" s="33"/>
-      <c r="K97" s="33"/>
+      <c r="G97" s="34"/>
+      <c r="H97" s="34"/>
+      <c r="I97" s="34"/>
+      <c r="J97" s="34"/>
+      <c r="K97" s="34"/>
     </row>
     <row r="98" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="21">
+      <c r="A98" s="11">
         <v>90</v>
       </c>
-      <c r="B98" s="36"/>
-      <c r="C98" s="34"/>
-      <c r="D98" s="34"/>
-      <c r="E98" s="31" t="s">
+      <c r="B98" s="23"/>
+      <c r="C98" s="22"/>
+      <c r="D98" s="22"/>
+      <c r="E98" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="F98" s="31" t="s">
+      <c r="F98" s="21" t="s">
         <v>57</v>
       </c>
       <c r="G98" s="35"/>
@@ -3047,66 +3047,64 @@
     </row>
   </sheetData>
   <mergeCells count="142">
-    <mergeCell ref="G93:G95"/>
-    <mergeCell ref="H93:H95"/>
-    <mergeCell ref="I93:I95"/>
-    <mergeCell ref="J93:J95"/>
-    <mergeCell ref="K93:K95"/>
-    <mergeCell ref="G84:G86"/>
-    <mergeCell ref="H84:H86"/>
-    <mergeCell ref="I84:I86"/>
-    <mergeCell ref="J84:J86"/>
-    <mergeCell ref="K84:K86"/>
-    <mergeCell ref="G90:G92"/>
-    <mergeCell ref="H90:H92"/>
-    <mergeCell ref="I90:I92"/>
-    <mergeCell ref="J90:J92"/>
-    <mergeCell ref="K90:K92"/>
-    <mergeCell ref="G87:G89"/>
-    <mergeCell ref="H87:H89"/>
-    <mergeCell ref="I87:I89"/>
-    <mergeCell ref="J87:J89"/>
-    <mergeCell ref="K87:K89"/>
-    <mergeCell ref="G69:G71"/>
-    <mergeCell ref="H69:H71"/>
-    <mergeCell ref="I69:I71"/>
-    <mergeCell ref="J69:J71"/>
-    <mergeCell ref="K69:K71"/>
-    <mergeCell ref="G66:G68"/>
-    <mergeCell ref="H66:H68"/>
-    <mergeCell ref="I66:I68"/>
-    <mergeCell ref="J66:J68"/>
-    <mergeCell ref="K66:K68"/>
-    <mergeCell ref="G81:G83"/>
-    <mergeCell ref="H81:H83"/>
-    <mergeCell ref="I81:I83"/>
-    <mergeCell ref="J81:J83"/>
-    <mergeCell ref="K81:K83"/>
-    <mergeCell ref="G78:G80"/>
-    <mergeCell ref="H78:H80"/>
-    <mergeCell ref="I78:I80"/>
-    <mergeCell ref="J78:J80"/>
-    <mergeCell ref="K78:K80"/>
-    <mergeCell ref="G75:G77"/>
-    <mergeCell ref="H75:H77"/>
-    <mergeCell ref="I75:I77"/>
-    <mergeCell ref="J75:J77"/>
-    <mergeCell ref="K75:K77"/>
-    <mergeCell ref="G72:G74"/>
-    <mergeCell ref="H72:H74"/>
-    <mergeCell ref="I72:I74"/>
-    <mergeCell ref="J72:J74"/>
-    <mergeCell ref="K72:K74"/>
-    <mergeCell ref="G63:G65"/>
-    <mergeCell ref="H63:H65"/>
-    <mergeCell ref="I63:I65"/>
-    <mergeCell ref="J63:J65"/>
-    <mergeCell ref="K63:K65"/>
-    <mergeCell ref="G60:G62"/>
-    <mergeCell ref="H60:H62"/>
-    <mergeCell ref="I60:I62"/>
-    <mergeCell ref="J60:J62"/>
-    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="G96:G98"/>
+    <mergeCell ref="H96:H98"/>
+    <mergeCell ref="I96:I98"/>
+    <mergeCell ref="J96:J98"/>
+    <mergeCell ref="K96:K98"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="H14:H16"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="K14:K16"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="G19:G21"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="J19:J21"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="G22:G24"/>
+    <mergeCell ref="H22:H24"/>
+    <mergeCell ref="I22:I24"/>
+    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="K22:K24"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="G28:G30"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="I28:I30"/>
+    <mergeCell ref="J28:J30"/>
+    <mergeCell ref="K28:K30"/>
+    <mergeCell ref="G31:G33"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="I31:I33"/>
+    <mergeCell ref="J31:J33"/>
+    <mergeCell ref="K31:K33"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="H34:H36"/>
+    <mergeCell ref="I34:I36"/>
+    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="K34:K36"/>
+    <mergeCell ref="I46:I48"/>
+    <mergeCell ref="J46:J48"/>
+    <mergeCell ref="K46:K48"/>
+    <mergeCell ref="G37:G39"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="K37:K39"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="J40:J42"/>
+    <mergeCell ref="K40:K42"/>
     <mergeCell ref="G55:G57"/>
     <mergeCell ref="H55:H57"/>
     <mergeCell ref="I55:I57"/>
@@ -3131,64 +3129,66 @@
     <mergeCell ref="K43:K45"/>
     <mergeCell ref="G46:G48"/>
     <mergeCell ref="H46:H48"/>
-    <mergeCell ref="I46:I48"/>
-    <mergeCell ref="J46:J48"/>
-    <mergeCell ref="K46:K48"/>
-    <mergeCell ref="G37:G39"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="K37:K39"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H40:H42"/>
-    <mergeCell ref="I40:I42"/>
-    <mergeCell ref="J40:J42"/>
-    <mergeCell ref="K40:K42"/>
-    <mergeCell ref="G31:G33"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="I31:I33"/>
-    <mergeCell ref="J31:J33"/>
-    <mergeCell ref="K31:K33"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="H34:H36"/>
-    <mergeCell ref="I34:I36"/>
-    <mergeCell ref="J34:J36"/>
-    <mergeCell ref="K34:K36"/>
-    <mergeCell ref="K22:K24"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="H25:H27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="G28:G30"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="I28:I30"/>
-    <mergeCell ref="J28:J30"/>
-    <mergeCell ref="K28:K30"/>
-    <mergeCell ref="G96:G98"/>
-    <mergeCell ref="H96:H98"/>
-    <mergeCell ref="I96:I98"/>
-    <mergeCell ref="J96:J98"/>
-    <mergeCell ref="K96:K98"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="H14:H16"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="K14:K16"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="J19:J21"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="G22:G24"/>
-    <mergeCell ref="H22:H24"/>
-    <mergeCell ref="I22:I24"/>
-    <mergeCell ref="J22:J24"/>
+    <mergeCell ref="G63:G65"/>
+    <mergeCell ref="H63:H65"/>
+    <mergeCell ref="I63:I65"/>
+    <mergeCell ref="J63:J65"/>
+    <mergeCell ref="K63:K65"/>
+    <mergeCell ref="G60:G62"/>
+    <mergeCell ref="H60:H62"/>
+    <mergeCell ref="I60:I62"/>
+    <mergeCell ref="J60:J62"/>
+    <mergeCell ref="K60:K62"/>
+    <mergeCell ref="G75:G77"/>
+    <mergeCell ref="H75:H77"/>
+    <mergeCell ref="I75:I77"/>
+    <mergeCell ref="J75:J77"/>
+    <mergeCell ref="K75:K77"/>
+    <mergeCell ref="G72:G74"/>
+    <mergeCell ref="H72:H74"/>
+    <mergeCell ref="I72:I74"/>
+    <mergeCell ref="J72:J74"/>
+    <mergeCell ref="K72:K74"/>
+    <mergeCell ref="G81:G83"/>
+    <mergeCell ref="H81:H83"/>
+    <mergeCell ref="I81:I83"/>
+    <mergeCell ref="J81:J83"/>
+    <mergeCell ref="K81:K83"/>
+    <mergeCell ref="G78:G80"/>
+    <mergeCell ref="H78:H80"/>
+    <mergeCell ref="I78:I80"/>
+    <mergeCell ref="J78:J80"/>
+    <mergeCell ref="K78:K80"/>
+    <mergeCell ref="G69:G71"/>
+    <mergeCell ref="H69:H71"/>
+    <mergeCell ref="I69:I71"/>
+    <mergeCell ref="J69:J71"/>
+    <mergeCell ref="K69:K71"/>
+    <mergeCell ref="G66:G68"/>
+    <mergeCell ref="H66:H68"/>
+    <mergeCell ref="I66:I68"/>
+    <mergeCell ref="J66:J68"/>
+    <mergeCell ref="K66:K68"/>
+    <mergeCell ref="G93:G95"/>
+    <mergeCell ref="H93:H95"/>
+    <mergeCell ref="I93:I95"/>
+    <mergeCell ref="J93:J95"/>
+    <mergeCell ref="K93:K95"/>
+    <mergeCell ref="G84:G86"/>
+    <mergeCell ref="H84:H86"/>
+    <mergeCell ref="I84:I86"/>
+    <mergeCell ref="J84:J86"/>
+    <mergeCell ref="K84:K86"/>
+    <mergeCell ref="G90:G92"/>
+    <mergeCell ref="H90:H92"/>
+    <mergeCell ref="I90:I92"/>
+    <mergeCell ref="J90:J92"/>
+    <mergeCell ref="K90:K92"/>
+    <mergeCell ref="G87:G89"/>
+    <mergeCell ref="H87:H89"/>
+    <mergeCell ref="I87:I89"/>
+    <mergeCell ref="J87:J89"/>
+    <mergeCell ref="K87:K89"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>